<commit_message>
PLL Board: Added datasheets, Completed PLL Board Schematics, Updated BOM.
</commit_message>
<xml_diff>
--- a/PLL_Board/PLL_PCB_BOM.xlsx
+++ b/PLL_Board/PLL_PCB_BOM.xlsx
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -267,9 +267,6 @@
     <t>Replaced lm358 with lm158 for greater temp range, 2 amps/chip</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>R21</t>
   </si>
   <si>
@@ -321,9 +318,6 @@
     <t>CR1</t>
   </si>
   <si>
-    <t>LED - Optional?</t>
-  </si>
-  <si>
     <t>C10</t>
   </si>
   <si>
@@ -351,12 +345,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>PLL 2211</t>
-  </si>
-  <si>
-    <t>N/L????</t>
-  </si>
-  <si>
     <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=445-5114-1-ND</t>
   </si>
   <si>
@@ -484,6 +472,51 @@
   </si>
   <si>
     <t>Sean choose a part, but it could not be located in eagle</t>
+  </si>
+  <si>
+    <t>XR221A</t>
+  </si>
+  <si>
+    <t>XR-2211A FSK Tone Decoder</t>
+  </si>
+  <si>
+    <t>1016-1309-5-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T93XA-50K-ND </t>
+  </si>
+  <si>
+    <t>T93YA-10K-ND  </t>
+  </si>
+  <si>
+    <t>http://www.newark.com/osram/lsr976-z/led-lamp/dp/97K3887?Ntt=LSR976-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSR976-Z </t>
+  </si>
+  <si>
+    <t>LED - RED</t>
+  </si>
+  <si>
+    <t>T93XA503KT20</t>
+  </si>
+  <si>
+    <t>T93YA103KT20</t>
+  </si>
+  <si>
+    <t>generic 0805 resistor</t>
+  </si>
+  <si>
+    <t>WM4800-ND</t>
+  </si>
+  <si>
+    <t>J1, J2, J3</t>
+  </si>
+  <si>
+    <t>70543-0001</t>
+  </si>
+  <si>
+    <t>2-Pin Vertical Connector, Pitch 0.100</t>
   </si>
 </sst>
 </file>
@@ -493,7 +526,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +579,19 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -670,11 +716,10 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -700,188 +745,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -906,25 +779,201 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H27" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H27" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:H27"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Reference Designator" dataDxfId="7"/>
-    <tableColumn id="2" name="Part Number" dataDxfId="6"/>
-    <tableColumn id="3" name="Description" dataDxfId="5"/>
-    <tableColumn id="4" name="Quantity per board" dataDxfId="4"/>
-    <tableColumn id="5" name="Price per Piece" dataDxfId="3"/>
-    <tableColumn id="6" name="Total Price" dataDxfId="2">
+    <tableColumn id="1" name="Reference Designator" dataDxfId="13"/>
+    <tableColumn id="2" name="Part Number" dataDxfId="12"/>
+    <tableColumn id="3" name="Description" dataDxfId="11"/>
+    <tableColumn id="4" name="Quantity per board" dataDxfId="10"/>
+    <tableColumn id="5" name="Price per Piece" dataDxfId="9"/>
+    <tableColumn id="6" name="Total Price" dataDxfId="8">
       <calculatedColumnFormula>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Link to vendor website" dataDxfId="1"/>
-    <tableColumn id="8" name="Notes" dataDxfId="0"/>
+    <tableColumn id="7" name="Link to vendor website" dataDxfId="7"/>
+    <tableColumn id="8" name="Notes" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1215,17 +1264,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
@@ -1234,82 +1283,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="47.25" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="16" t="s">
-        <v>45</v>
-      </c>
+      <c r="A2" s="15"/>
       <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
         <v>0.63</v>
       </c>
-      <c r="F2" s="7">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0.63</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>81</v>
+      <c r="F2" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>5</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>0.33800000000000002</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>1.6900000000000002</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1317,7 +1364,7 @@
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1326,17 +1373,17 @@
       <c r="D4" s="1">
         <v>6</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>0.27</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>1.62</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1344,97 +1391,101 @@
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>0.09</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.09</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>93</v>
+      <c r="G5" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="1">
         <v>4</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>0.33</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>1.32</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7">
+      <c r="A7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="12" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>0.47699999999999998</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.95399999999999996</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1442,26 +1493,26 @@
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1469,481 +1520,544 @@
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>0.1</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.1</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>84</v>
+      <c r="G11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>1.84</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>1.84</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>0.1</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.2</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" s="13" t="s">
+      <c r="G13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>0.1</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.1</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="13" t="s">
+      <c r="G14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>0.1</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.1</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="13" t="s">
+      <c r="G15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>0.1</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.2</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>57</v>
+      <c r="C17" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>8.02</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>8.02</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>99</v>
+      <c r="G17" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>0.1</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.1</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" s="13" t="s">
+      <c r="G18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>0.1</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0.1</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="13" t="s">
+      <c r="G19" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F20" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="B21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>65</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>8</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>8</v>
       </c>
-      <c r="G21" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="16" t="s">
+      <c r="G21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75">
+      <c r="A22" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="F22" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>1.7</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="12" t="s">
+      <c r="B23" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>69</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>7.24</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>7.24</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" s="20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="16" t="s">
+      <c r="G23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75">
+      <c r="A24" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1.7</v>
+      </c>
+      <c r="F24" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>1.7</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="18" t="s">
+      <c r="B25" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="20">
+        <v>1</v>
+      </c>
+      <c r="E25" s="24">
+        <v>2.65</v>
+      </c>
+      <c r="F25" s="24">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>2.65</v>
+      </c>
+      <c r="G25" s="25" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" s="11" customFormat="1">
-      <c r="A26" s="19" t="s">
+      <c r="H25" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="10" customFormat="1">
+      <c r="A26" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>107</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>111</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>0.52</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>1.04</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7">
+      <c r="D27" s="11">
+        <v>2</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
         <v>0</v>
       </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="9" t="s">
+      <c r="G27" s="14"/>
+      <c r="H27" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="10" customFormat="1">
+      <c r="A28" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="11">
+        <v>3</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="F28" s="6">
+        <f>D28*E28</f>
+        <v>2.9699999999999998</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="H28" s="21"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <f>SUM(Table1[Quantity per board])</f>
-        <v>36</v>
-      </c>
-      <c r="F28" s="8">
+        <v>42</v>
+      </c>
+      <c r="F29" s="7">
         <f>SUM(Table1[Total Price])</f>
-        <v>33.475999999999999</v>
-      </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="C30" s="11"/>
+        <v>38.953000000000003</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3">
-      <c r="C33" s="11" t="s">
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="C34" s="10" t="s">
         <v>28</v>
       </c>
+      <c r="G34" s="22" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="F29">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1968,12 +2082,18 @@
     <hyperlink ref="G18" r:id="rId18"/>
     <hyperlink ref="G19" r:id="rId19"/>
     <hyperlink ref="G26" r:id="rId20"/>
+    <hyperlink ref="G25" r:id="rId21" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=1016-1309-5-ND"/>
+    <hyperlink ref="G22" r:id="rId22" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=T93XA-50K-ND"/>
+    <hyperlink ref="G24" r:id="rId23" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=T93YA-10K-ND"/>
+    <hyperlink ref="G20" r:id="rId24"/>
+    <hyperlink ref="G34" r:id="rId25" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM4800-ND"/>
+    <hyperlink ref="G28" r:id="rId26" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM4800-ND"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="301" verticalDpi="300" r:id="rId21"/>
-  <legacyDrawing r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="301" verticalDpi="300" r:id="rId27"/>
+  <legacyDrawing r:id="rId28"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added noise mat files for dylan
</commit_message>
<xml_diff>
--- a/PLL_Board/PLL_PCB_BOM.xlsx
+++ b/PLL_Board/PLL_PCB_BOM.xlsx
@@ -19,31 +19,7 @@
     <author>Dylan Thorner</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dylan Thorner:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Can't find a footprint in Eagle… Not currently in schematic</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="125">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -355,18 +331,6 @@
   </si>
   <si>
     <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=490-1506-1-ND</t>
-  </si>
-  <si>
-    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=CP1-3513SJCT-ND</t>
-  </si>
-  <si>
-    <t>3.5 mm audio jack</t>
-  </si>
-  <si>
-    <t>3.5 mm audio jack for audio input from rockmite</t>
-  </si>
-  <si>
-    <t>CP1-3513SJCT-ND</t>
   </si>
   <si>
     <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=P430KFCT-ND</t>
@@ -780,49 +744,6 @@
       </fill>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -955,25 +876,68 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H27" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
-  <autoFilter ref="A1:H27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:H26"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Reference Designator" dataDxfId="13"/>
-    <tableColumn id="2" name="Part Number" dataDxfId="12"/>
-    <tableColumn id="3" name="Description" dataDxfId="11"/>
-    <tableColumn id="4" name="Quantity per board" dataDxfId="10"/>
-    <tableColumn id="5" name="Price per Piece" dataDxfId="9"/>
-    <tableColumn id="6" name="Total Price" dataDxfId="8">
+    <tableColumn id="1" name="Reference Designator" dataDxfId="9"/>
+    <tableColumn id="2" name="Part Number" dataDxfId="8"/>
+    <tableColumn id="3" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" name="Quantity per board" dataDxfId="6"/>
+    <tableColumn id="5" name="Price per Piece" dataDxfId="5"/>
+    <tableColumn id="6" name="Total Price" dataDxfId="4">
       <calculatedColumnFormula>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Link to vendor website" dataDxfId="7"/>
-    <tableColumn id="8" name="Notes" dataDxfId="6"/>
+    <tableColumn id="7" name="Link to vendor website" dataDxfId="3"/>
+    <tableColumn id="8" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1264,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1309,313 +1273,315 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="15"/>
-      <c r="B2" t="s">
-        <v>78</v>
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E2" s="6">
-        <v>0.63</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="F2" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0</v>
+        <v>1.6900000000000002</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D3" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="6">
-        <v>0.33800000000000002</v>
+        <v>0.27</v>
       </c>
       <c r="F3" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>1.6900000000000002</v>
+        <v>1.62</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>86</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="D4" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6">
-        <v>0.27</v>
+        <v>0.09</v>
       </c>
       <c r="F4" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>1.62</v>
+        <v>0.09</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
+      <c r="A5" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="F5" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>1.32</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
-        <v>0.09</v>
-      </c>
-      <c r="F5" s="6">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0.09</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.33</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>1.32</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G6" s="14"/>
       <c r="H6" s="12" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="11"/>
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="11" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.47699999999999998</v>
+      </c>
       <c r="F7" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="12" t="s">
-        <v>124</v>
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>0.47699999999999998</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="F8" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0.95399999999999996</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="6">
-        <v>8.6999999999999994E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F9" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>8.6999999999999994E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
+      <c r="A10" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="6">
-        <v>4.4999999999999998E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F10" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>4.4999999999999998E-2</v>
+        <v>0.1</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>33</v>
+        <v>75</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="18" t="s">
-        <v>46</v>
+      <c r="A11" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="6">
+        <v>1.84</v>
+      </c>
+      <c r="F11" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>1.84</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="6">
         <v>0.1</v>
       </c>
-      <c r="F11" s="6">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0.1</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1.84</v>
-      </c>
       <c r="F12" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>1.84</v>
+        <v>0.2</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
         <v>83</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="6">
         <v>0.1</v>
       </c>
       <c r="F13" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>82</v>
@@ -1626,13 +1592,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>87</v>
+        <v>52</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1645,7 +1611,7 @@
         <v>0.1</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>39</v>
@@ -1653,26 +1619,26 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="6">
         <v>0.1</v>
       </c>
       <c r="F15" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>39</v>
@@ -1680,67 +1646,67 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="18" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <v>8.02</v>
+      </c>
+      <c r="F16" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>8.02</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="F16" s="6">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="C17" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="6">
-        <v>8.02</v>
+        <v>0.1</v>
       </c>
       <c r="F17" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>8.02</v>
+        <v>0.1</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>95</v>
+      <c r="H17" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -1753,7 +1719,7 @@
         <v>0.1</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>39</v>
@@ -1761,299 +1727,272 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>99</v>
+        <v>61</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="6">
-        <v>0.1</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F19" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0.1</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>120</v>
+        <v>62</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="6">
-        <v>5.7000000000000002E-2</v>
+        <v>8</v>
       </c>
       <c r="F20" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>5.7000000000000002E-2</v>
+        <v>8</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>71</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75">
       <c r="A21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>118</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="6">
-        <v>8</v>
+        <v>1.7</v>
       </c>
       <c r="F21" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>8</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75">
+        <v>1.7</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>122</v>
+        <v>66</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="6">
-        <v>1.7</v>
+        <v>7.24</v>
       </c>
       <c r="F22" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>1.7</v>
-      </c>
-      <c r="G22" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>7.24</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75">
       <c r="A23" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>119</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="6">
-        <v>7.24</v>
+        <v>1.7</v>
       </c>
       <c r="F23" s="6">
         <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>7.24</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H23" s="19" t="s">
+        <v>1.7</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="20">
+        <v>1</v>
+      </c>
+      <c r="E24" s="24">
+        <v>2.65</v>
+      </c>
+      <c r="F24" s="24">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>2.65</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="10" customFormat="1">
+      <c r="A25" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.52</v>
+      </c>
+      <c r="F25" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>1.04</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75">
-      <c r="A24" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="23" t="s">
+    <row r="26" spans="1:8">
+      <c r="A26" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6">
+        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="10" customFormat="1">
+      <c r="A27" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1.7</v>
-      </c>
-      <c r="F24" s="6">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>1.7</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="20">
-        <v>1</v>
-      </c>
-      <c r="E25" s="24">
-        <v>2.65</v>
-      </c>
-      <c r="F25" s="24">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>2.65</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="10" customFormat="1">
-      <c r="A26" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2</v>
-      </c>
-      <c r="E26" s="6">
-        <v>0.52</v>
-      </c>
-      <c r="F26" s="6">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>1.04</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="11"/>
       <c r="C27" s="11" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D27" s="11">
-        <v>2</v>
-      </c>
-      <c r="E27" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.99</v>
+      </c>
       <c r="F27" s="6">
-        <f>Table1[[#This Row],[Quantity per board]]*Table1[[#This Row],[Price per Piece]]</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="10" customFormat="1">
-      <c r="A28" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="11">
-        <v>3</v>
-      </c>
-      <c r="E28" s="6">
-        <v>0.99</v>
-      </c>
-      <c r="F28" s="6">
-        <f>D28*E28</f>
+        <f>D27*E27</f>
         <v>2.9699999999999998</v>
       </c>
-      <c r="G28" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="H28" s="21"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="8" t="s">
+      <c r="G27" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D29">
+      <c r="D28">
         <f>SUM(Table1[Quantity per board])</f>
         <v>42</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F28" s="7">
         <f>SUM(Table1[Total Price])</f>
         <v>38.953000000000003</v>
       </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="3:7">
-      <c r="C34" s="10" t="s">
+      <c r="A31" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="22" t="s">
-        <v>125</v>
+      <c r="G33" s="22" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F29">
+  <conditionalFormatting sqref="F28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>40</formula>
     </cfRule>
@@ -2062,38 +2001,37 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G6" r:id="rId2"/>
-    <hyperlink ref="G8" r:id="rId3"/>
-    <hyperlink ref="G10" r:id="rId4"/>
-    <hyperlink ref="G4" r:id="rId5"/>
-    <hyperlink ref="G9" r:id="rId6"/>
-    <hyperlink ref="G12" r:id="rId7"/>
-    <hyperlink ref="G21" r:id="rId8"/>
-    <hyperlink ref="G23" r:id="rId9"/>
-    <hyperlink ref="G2" r:id="rId10"/>
-    <hyperlink ref="G11" r:id="rId11"/>
-    <hyperlink ref="G13" r:id="rId12"/>
-    <hyperlink ref="G15" r:id="rId13"/>
-    <hyperlink ref="G14" r:id="rId14"/>
-    <hyperlink ref="G5" r:id="rId15"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G7" r:id="rId3"/>
+    <hyperlink ref="G9" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G11" r:id="rId7"/>
+    <hyperlink ref="G20" r:id="rId8"/>
+    <hyperlink ref="G22" r:id="rId9"/>
+    <hyperlink ref="G10" r:id="rId10"/>
+    <hyperlink ref="G12" r:id="rId11"/>
+    <hyperlink ref="G14" r:id="rId12"/>
+    <hyperlink ref="G13" r:id="rId13"/>
+    <hyperlink ref="G4" r:id="rId14"/>
+    <hyperlink ref="G15" r:id="rId15"/>
     <hyperlink ref="G16" r:id="rId16"/>
     <hyperlink ref="G17" r:id="rId17"/>
     <hyperlink ref="G18" r:id="rId18"/>
-    <hyperlink ref="G19" r:id="rId19"/>
-    <hyperlink ref="G26" r:id="rId20"/>
-    <hyperlink ref="G25" r:id="rId21" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=1016-1309-5-ND"/>
-    <hyperlink ref="G22" r:id="rId22" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=T93XA-50K-ND"/>
-    <hyperlink ref="G24" r:id="rId23" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=T93YA-10K-ND"/>
-    <hyperlink ref="G20" r:id="rId24"/>
-    <hyperlink ref="G34" r:id="rId25" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM4800-ND"/>
-    <hyperlink ref="G28" r:id="rId26" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM4800-ND"/>
+    <hyperlink ref="G25" r:id="rId19"/>
+    <hyperlink ref="G24" r:id="rId20" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=1016-1309-5-ND"/>
+    <hyperlink ref="G21" r:id="rId21" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=T93XA-50K-ND"/>
+    <hyperlink ref="G23" r:id="rId22" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=T93YA-10K-ND"/>
+    <hyperlink ref="G19" r:id="rId23"/>
+    <hyperlink ref="G33" r:id="rId24" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM4800-ND"/>
+    <hyperlink ref="G27" r:id="rId25" display="http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM4800-ND"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="301" verticalDpi="300" r:id="rId27"/>
-  <legacyDrawing r:id="rId28"/>
+  <pageSetup orientation="portrait" horizontalDpi="301" verticalDpi="300" r:id="rId26"/>
+  <legacyDrawing r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>